<commit_message>
second commit for hotspot pom framwork
</commit_message>
<xml_diff>
--- a/src/main/java/com/hubspot/qa/util/HubSpotData 2.xlsx
+++ b/src/main/java/com/hubspot/qa/util/HubSpotData 2.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="19014" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="16164" windowHeight="2856" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Username</t>
   </si>
@@ -100,6 +101,30 @@
   </si>
   <si>
     <t>Developer</t>
+  </si>
+  <si>
+    <t>DealName</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Sun Islam</t>
+  </si>
+  <si>
+    <t>shobuj Alam200</t>
+  </si>
+  <si>
+    <t>Badsha Alam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazmul </t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+  <si>
+    <t>Jewal</t>
   </si>
 </sst>
 </file>
@@ -451,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -575,12 +600,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.3671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>